<commit_message>
Actualización 8 de marzo de 2024 - Lap HP
Se actualiza el repositorio.
</commit_message>
<xml_diff>
--- a/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Laboratorio_Parcial_03_NRC_126.xlsx
+++ b/Bitacoras/NRC_124_Grupo_43/Parcial_03/Bitacora_Laboratorio_Parcial_03_NRC_126.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Plan PU\Fisica_3\Bitacoras\NRC_124_Grupo_43\Parcial_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F90C92C-B515-4091-81EC-4E7E12A47200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F82CC09-F518-4F7A-8708-96086130B924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D7C6AF72-9BA1-470B-9C11-141FBCE526C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D7C6AF72-9BA1-470B-9C11-141FBCE526C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Faltas" sheetId="1" r:id="rId1"/>
     <sheet name="Concentrado" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Concentrado!$A$2:$R$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
   <si>
     <t>Alumno</t>
   </si>
@@ -213,9 +216,6 @@
     <t>P5_Montaje</t>
   </si>
   <si>
-    <t>P5_Marco_Teórico</t>
-  </si>
-  <si>
     <t>P5_Reporte</t>
   </si>
   <si>
@@ -247,14 +247,31 @@
   </si>
   <si>
     <t>Baja</t>
+  </si>
+  <si>
+    <t>P5_Marco</t>
+  </si>
+  <si>
+    <t>P7_Marco</t>
+  </si>
+  <si>
+    <t>P6_Marco</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -288,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,11 +317,48 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -634,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D9BAF7-11AE-4343-ACC0-8FC082EA6C8D}">
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,10 +699,11 @@
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="6.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -679,11 +734,14 @@
       <c r="J1" s="1">
         <v>45341</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K1" s="1">
+        <v>45348</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -699,12 +757,12 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f>SUM(E2:J2)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -717,12 +775,12 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="2">
-        <f t="shared" ref="K3:K16" si="0">SUM(E3:J3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="2">
+        <f t="shared" ref="L3:L16" si="0">SUM(E3:J3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -742,11 +800,14 @@
         <v>1</v>
       </c>
       <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -759,12 +820,12 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -777,12 +838,12 @@
       <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -795,12 +856,12 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -813,12 +874,12 @@
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -831,12 +892,12 @@
       <c r="D9" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -849,12 +910,12 @@
       <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -870,12 +931,21 @@
       <c r="H11" s="2">
         <v>1</v>
       </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
       <c r="K11" s="2">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="2">
+        <f>SUM(E11:K11)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -888,12 +958,12 @@
       <c r="D12" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -906,12 +976,12 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -928,11 +998,14 @@
         <v>1</v>
       </c>
       <c r="K14" s="2">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -945,12 +1018,12 @@
       <c r="D15" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>52</v>
       </c>
@@ -975,12 +1048,13 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>69</v>
+      <c r="M16" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -990,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3911F978-7D9C-4295-B748-1C60794BFA1E}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,356 +1075,484 @@
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E1" s="2">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2">
+        <v>5</v>
+      </c>
+      <c r="K1" s="2">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2">
+        <v>5</v>
+      </c>
+      <c r="N1" s="2">
+        <v>5</v>
+      </c>
+      <c r="O1" s="2">
+        <v>5</v>
+      </c>
+      <c r="P1" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="2">
+        <f>SUM(E1:P1)</f>
+        <v>60</v>
+      </c>
+      <c r="R1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="2">
-        <v>5</v>
-      </c>
-      <c r="K2" s="2">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2">
-        <f>SUM(E2:L2)</f>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>5</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>SUM(E3:P3)</f>
+        <v>25</v>
+      </c>
+      <c r="R3" s="6">
+        <f>(Q3/$Q$1)*10</f>
+        <v>4.166666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>5</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>5</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>5</v>
+      </c>
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:Q17" si="0">SUM(E4:P4)</f>
+        <v>30</v>
+      </c>
+      <c r="R4" s="6">
+        <f t="shared" ref="R4:R16" si="1">(Q4/$Q$1)*10</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>5</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>5</v>
-      </c>
-      <c r="K3" s="2">
-        <v>5</v>
-      </c>
-      <c r="O3" s="2">
-        <f t="shared" ref="O3:O15" si="0">SUM(E3:L3)</f>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>5</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>5</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>5</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>5</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>5</v>
-      </c>
-      <c r="O4" s="2">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="R5" s="6">
+        <f t="shared" si="1"/>
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>5</v>
-      </c>
-      <c r="I5" s="2">
-        <v>4</v>
-      </c>
-      <c r="J5" s="2">
-        <v>5</v>
-      </c>
-      <c r="K5" s="2">
-        <v>5</v>
-      </c>
-      <c r="O5" s="2">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>5</v>
+      </c>
+      <c r="H6" s="2">
+        <v>5</v>
+      </c>
+      <c r="I6" s="2">
+        <v>4</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>5</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="R6" s="6">
+        <f t="shared" si="1"/>
+        <v>7.833333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="R7" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>5</v>
-      </c>
-      <c r="I7" s="2">
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>5</v>
+      </c>
+      <c r="I8" s="2">
         <v>3</v>
       </c>
-      <c r="J7" s="2">
-        <v>5</v>
-      </c>
-      <c r="K7" s="2">
-        <v>5</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2">
+        <v>3</v>
+      </c>
+      <c r="L8" s="2">
+        <v>5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3</v>
+      </c>
+      <c r="N8" s="2">
+        <v>5</v>
+      </c>
+      <c r="O8" s="2">
+        <v>5</v>
+      </c>
+      <c r="P8" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="R8" s="6">
+        <f t="shared" si="1"/>
+        <v>7.333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="F8" s="2">
-        <v>5</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>5</v>
-      </c>
-      <c r="I8" s="2">
-        <v>5</v>
-      </c>
-      <c r="J8" s="2">
-        <v>5</v>
-      </c>
-      <c r="K8" s="2">
-        <v>5</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="0"/>
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9" s="2">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
@@ -1362,148 +1564,224 @@
         <v>5</v>
       </c>
       <c r="I9" s="2">
+        <v>5</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5</v>
+      </c>
+      <c r="K9" s="2">
         <v>4.5</v>
       </c>
-      <c r="J9" s="2">
-        <v>5</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
+        <v>5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2">
         <v>5</v>
       </c>
       <c r="O9" s="2">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="P9" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="R9" s="6">
+        <f t="shared" si="1"/>
+        <v>9.8333333333333321</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J10" s="2">
+        <v>5</v>
+      </c>
+      <c r="K10" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="L10" s="2">
+        <v>5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>4</v>
+      </c>
+      <c r="N10" s="2">
+        <v>5</v>
+      </c>
+      <c r="O10" s="2">
+        <v>5</v>
+      </c>
+      <c r="P10" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="0"/>
+        <v>55.5</v>
+      </c>
+      <c r="R10" s="6">
+        <f t="shared" si="1"/>
+        <v>9.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>5</v>
-      </c>
-      <c r="I10" s="2">
-        <v>5</v>
-      </c>
-      <c r="J10" s="2">
-        <v>5</v>
-      </c>
-      <c r="K10" s="2">
-        <v>5</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>5</v>
+      </c>
+      <c r="L11" s="2">
+        <v>5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="N11" s="2">
+        <v>5</v>
+      </c>
+      <c r="O11" s="2">
+        <v>5</v>
+      </c>
+      <c r="P11" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="R11" s="6">
+        <f t="shared" si="1"/>
+        <v>9.0833333333333339</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>37</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>5</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>5</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0</v>
-      </c>
-      <c r="J11" s="2">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>5</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R12" s="6">
+        <f t="shared" si="1"/>
+        <v>3.333333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
-        <v>5</v>
-      </c>
-      <c r="G12" s="2">
-        <v>5</v>
-      </c>
-      <c r="H12" s="2">
-        <v>5</v>
-      </c>
-      <c r="I12" s="2">
-        <v>5</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2">
-        <v>5</v>
-      </c>
-      <c r="O12" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" s="2">
         <v>5</v>
@@ -1526,132 +1804,273 @@
       <c r="K13" s="2">
         <v>5</v>
       </c>
+      <c r="L13" s="2">
+        <v>5</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2">
+        <v>5</v>
+      </c>
       <c r="O13" s="2">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="P13" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="R13" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
       </c>
       <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
+      <c r="H14" s="2">
+        <v>5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>5</v>
+      </c>
+      <c r="J14" s="2">
+        <v>5</v>
+      </c>
+      <c r="K14" s="2">
+        <v>5</v>
+      </c>
+      <c r="L14" s="2">
+        <v>5</v>
+      </c>
+      <c r="M14" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="N14" s="2">
+        <v>5</v>
+      </c>
+      <c r="O14" s="2">
+        <v>5</v>
+      </c>
+      <c r="P14" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="0"/>
+        <v>59.5</v>
+      </c>
+      <c r="R14" s="6">
+        <f t="shared" si="1"/>
+        <v>9.9166666666666679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="2">
         <v>2.5</v>
       </c>
-      <c r="F14" s="2">
-        <v>5</v>
-      </c>
-      <c r="G14" s="2">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2">
-        <v>5</v>
-      </c>
-      <c r="I14" s="2">
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>5</v>
+      </c>
+      <c r="I15" s="2">
         <v>4</v>
       </c>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
-        <v>5</v>
-      </c>
-      <c r="O14" s="2">
-        <f t="shared" si="0"/>
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>4</v>
+      </c>
+      <c r="L15" s="2">
+        <v>5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>5</v>
+      </c>
+      <c r="O15" s="2">
+        <v>5</v>
+      </c>
+      <c r="P15" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="0"/>
+        <v>45.5</v>
+      </c>
+      <c r="R15" s="6">
+        <f t="shared" si="1"/>
+        <v>7.583333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>49</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E16" s="2">
         <v>2</v>
       </c>
-      <c r="F15" s="2">
-        <v>5</v>
-      </c>
-      <c r="G15" s="2">
-        <v>5</v>
-      </c>
-      <c r="H15" s="2">
-        <v>5</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
-        <v>5</v>
-      </c>
-      <c r="K15" s="2">
-        <v>5</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>5</v>
+      </c>
+      <c r="K16" s="2">
+        <v>4</v>
+      </c>
+      <c r="L16" s="2">
+        <v>5</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0</v>
+      </c>
+      <c r="P16" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="R16" s="6">
+        <f t="shared" si="1"/>
+        <v>6.8333333333333339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P16" s="4"/>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>0</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:R17" xr:uid="{3911F978-7D9C-4295-B748-1C60794BFA1E}"/>
+  <conditionalFormatting sqref="E3:P3">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:P16">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>